<commit_message>
update code and results for 2015
</commit_message>
<xml_diff>
--- a/output/resultsummary.xlsx
+++ b/output/resultsummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yzz3363/Documents/Rstudio/UBRR/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F22152-E3CE-C943-B211-BD12352E7251}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D96E52-4478-7C43-A150-B18126EE0BED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{A4114632-EF87-9B4A-9301-938BFB9B362C}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="61">
   <si>
     <t>Urban</t>
   </si>
@@ -207,13 +207,16 @@
   </si>
   <si>
     <t>ER</t>
+  </si>
+  <si>
+    <t>rating</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +234,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -274,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -286,9 +295,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB45659A-0F08-1C42-BDBF-A87EBD364EFE}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection sqref="A1:H40"/>
+    <sheetView topLeftCell="A14" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1284,25 +1294,25 @@
       <c r="A36" t="s">
         <v>11</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="4">
         <v>63.553418471463402</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="4">
         <v>66</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="4">
         <v>19.361879641902899</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="4">
         <v>64.2013267832276</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="4">
         <v>66</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="4">
         <v>15.9907647520719</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="4">
         <v>9.7618667741756607E-2</v>
       </c>
     </row>
@@ -1694,280 +1704,838 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDB2D81-59B2-0D49-B33A-5E9C030744C6}">
-  <dimension ref="A2:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="142" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="B3">
+        <v>83</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="D3">
+        <v>140</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="B4">
+        <v>400</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D4">
+        <v>2111</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4.7E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="B5">
+        <v>747</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D5">
+        <v>4126</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9.0999999999999998E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="B6">
+        <v>49</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>313</v>
+      </c>
+      <c r="E6" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="B7">
+        <v>4234</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.7E-2</v>
+      </c>
+      <c r="D7">
+        <v>4007</v>
+      </c>
+      <c r="E7" s="2">
+        <v>8.8999999999999996E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="B8">
+        <v>6830</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D8">
+        <v>4578</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.10100000000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="B9">
+        <v>3384</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D9">
+        <v>2016</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4.4999999999999998E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="B10">
+        <v>550</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D10">
+        <v>517</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="B11">
+        <v>878</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D11">
+        <v>660</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="B12">
+        <v>138911</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="D12">
+        <v>25710</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.56899999999999995</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="B13">
+        <v>460</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D13">
+        <v>281</v>
+      </c>
+      <c r="E13" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="B14">
+        <v>116</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="D14">
+        <v>672</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="B17">
+        <v>156652</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>45147</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="B18">
+        <v>152192</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="D18">
+        <v>44101</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.97699999999999998</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="B19">
+        <v>148480</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="D19">
+        <v>39782</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.88100000000000001</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
+      <c r="B20">
+        <v>142032</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="D20" s="8">
+        <v>37909</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0.84</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
+      <c r="B21">
+        <v>138583</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="D21" s="8">
+        <v>32563</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0.72099999999999997</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="B22">
+        <v>149261</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="D22">
+        <v>43500</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.96399999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="B25">
+        <v>3.2722490154919099</v>
+      </c>
+      <c r="C25">
+        <v>3.5</v>
+      </c>
+      <c r="D25">
+        <v>0.91384187001764605</v>
+      </c>
+      <c r="E25">
+        <v>3.22495595107377</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>0.84351459261377904</v>
+      </c>
+      <c r="H25" s="12">
+        <v>2.5393876874931398E-28</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B26">
+        <v>91.454263947696603</v>
+      </c>
+      <c r="C26">
+        <v>94.3</v>
+      </c>
+      <c r="D26">
+        <v>9.0778585404389194</v>
+      </c>
+      <c r="E26">
+        <v>92.967763269049698</v>
+      </c>
+      <c r="F26">
+        <v>95</v>
+      </c>
+      <c r="G26">
+        <v>6.9702201352135802</v>
+      </c>
+      <c r="H26" s="12">
+        <v>4.9218123695859701E-88</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>95.270180380174907</v>
+      </c>
+      <c r="C27">
+        <v>98.2</v>
+      </c>
+      <c r="D27">
+        <v>8.9345912865725197</v>
+      </c>
+      <c r="E27">
+        <v>95.024538558175493</v>
+      </c>
+      <c r="F27">
+        <v>98</v>
+      </c>
+      <c r="G27">
+        <v>8.4565946197789206</v>
+      </c>
+      <c r="H27" s="12">
+        <v>2.98334009466628E-31</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="B28" s="4">
+        <v>99.074193416945803</v>
+      </c>
+      <c r="C28" s="4">
+        <v>100</v>
+      </c>
+      <c r="D28" s="4">
+        <v>3.1108727068229398</v>
+      </c>
+      <c r="E28" s="4">
+        <v>99.182610176087195</v>
+      </c>
+      <c r="F28" s="4">
+        <v>100</v>
+      </c>
+      <c r="G28" s="4">
+        <v>2.9872754028349</v>
+      </c>
+      <c r="H28" s="13">
+        <v>0.216159466260893</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>22</v>
-      </c>
-      <c r="H29" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="B29" s="8">
+        <v>96.355300191721795</v>
+      </c>
+      <c r="C29" s="8">
+        <v>99.1</v>
+      </c>
+      <c r="D29" s="8">
+        <v>9.1263114889419494</v>
+      </c>
+      <c r="E29" s="8">
+        <v>97.384714375392306</v>
+      </c>
+      <c r="F29" s="8">
+        <v>99.2</v>
+      </c>
+      <c r="G29" s="8">
+        <v>6.19621181407219</v>
+      </c>
+      <c r="H29" s="12">
+        <v>1.6782358343141601E-7</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="B30">
+        <v>69.343314839350796</v>
+      </c>
+      <c r="C30">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="D30">
+        <v>21.169077474322499</v>
+      </c>
+      <c r="E30">
+        <v>72.849636570411406</v>
+      </c>
+      <c r="F30">
+        <v>75</v>
+      </c>
+      <c r="G30">
+        <v>14.1654786397433</v>
+      </c>
+      <c r="H30" s="12">
+        <v>4.3414211575095402E-24</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="B31" s="5">
+        <v>70.7758549942521</v>
+      </c>
+      <c r="C31" s="5">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="D31" s="5">
+        <v>24.046433548327901</v>
+      </c>
+      <c r="E31" s="8">
+        <v>78.139951128638103</v>
+      </c>
+      <c r="F31" s="8">
+        <v>81.8</v>
+      </c>
+      <c r="G31" s="8">
+        <v>15.856362738625799</v>
+      </c>
+      <c r="H31" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="B32">
+        <v>96.050952497974905</v>
+      </c>
+      <c r="C32">
+        <v>98.7</v>
+      </c>
+      <c r="D32">
+        <v>7.9856218711001796</v>
+      </c>
+      <c r="E32">
+        <v>95.793430036396501</v>
+      </c>
+      <c r="F32">
+        <v>98.4</v>
+      </c>
+      <c r="G32">
+        <v>7.4634295173653298</v>
+      </c>
+      <c r="H32" s="12">
+        <v>5.2406310725796298E-70</v>
+      </c>
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="B33" s="4">
+        <v>78.686790228509594</v>
+      </c>
+      <c r="C33" s="4">
+        <v>78</v>
+      </c>
+      <c r="D33" s="4">
+        <v>17.7135424813453</v>
+      </c>
+      <c r="E33" s="4">
+        <v>79.471499908970301</v>
+      </c>
+      <c r="F33" s="4">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="G33" s="4">
+        <v>15.7377743287917</v>
+      </c>
+      <c r="H33" s="13">
+        <v>9.9273027227925997E-2</v>
+      </c>
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="13"/>
+        <v>8</v>
+      </c>
+      <c r="B34">
+        <v>77.039952766770497</v>
+      </c>
+      <c r="C34">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="D34">
+        <v>19.778975825934499</v>
+      </c>
+      <c r="E34">
+        <v>78.668630226766297</v>
+      </c>
+      <c r="F34">
+        <v>77.7</v>
+      </c>
+      <c r="G34">
+        <v>17.388356638718101</v>
+      </c>
+      <c r="H34" s="12">
+        <v>9.8387101766748302E-16</v>
+      </c>
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="B35" s="4">
+        <v>81.220988356531095</v>
+      </c>
+      <c r="C35" s="4">
+        <v>83.1</v>
+      </c>
+      <c r="D35" s="4">
+        <v>17.9641163040157</v>
+      </c>
+      <c r="E35" s="4">
+        <v>81.949885229540897</v>
+      </c>
+      <c r="F35" s="4">
+        <v>82.3</v>
+      </c>
+      <c r="G35" s="4">
+        <v>15.863349690609899</v>
+      </c>
+      <c r="H35" s="13">
+        <v>0.150824867260691</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B36" s="8">
+        <v>69.610340126542496</v>
+      </c>
+      <c r="C36" s="8">
+        <v>70.5</v>
+      </c>
+      <c r="D36" s="8">
+        <v>17.7860638596648</v>
+      </c>
+      <c r="E36" s="8">
+        <v>67.354884496919894</v>
+      </c>
+      <c r="F36" s="8">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="G36" s="8">
+        <v>14.479450251768</v>
+      </c>
+      <c r="H36" s="12">
+        <v>4.9444605371521801E-205</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B37" s="4">
+        <v>64.843618231592401</v>
+      </c>
+      <c r="C37" s="4">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="D37" s="4">
+        <v>19.1107068522277</v>
+      </c>
+      <c r="E37" s="11">
+        <v>65.596249934531002</v>
+      </c>
+      <c r="F37" s="11">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="G37" s="11">
+        <v>15.815118630427801</v>
+      </c>
+      <c r="H37" s="13">
+        <v>0.782953964607078</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="H38" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="B38">
+        <v>77.377228755299996</v>
+      </c>
+      <c r="C38">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="D38">
+        <v>17.714495649809301</v>
+      </c>
+      <c r="E38">
+        <v>79.182095205003506</v>
+      </c>
+      <c r="F38">
+        <v>82.6</v>
+      </c>
+      <c r="G38">
+        <v>15.9803560955175</v>
+      </c>
+      <c r="H38" s="12">
+        <v>1.4347301088923299E-28</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="B39">
+        <v>56.189279948625099</v>
+      </c>
+      <c r="C39">
+        <v>57.2</v>
+      </c>
+      <c r="D39">
+        <v>16.8511359924929</v>
+      </c>
+      <c r="E39">
+        <v>57.1926834442706</v>
+      </c>
+      <c r="F39">
+        <v>57.5</v>
+      </c>
+      <c r="G39">
+        <v>13.900060681380699</v>
+      </c>
+      <c r="H39" s="12">
+        <v>1.7972463853668099E-11</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40">
+        <v>11.857792141552199</v>
+      </c>
+      <c r="C40">
+        <v>11.8</v>
+      </c>
+      <c r="D40">
+        <v>4.1208161771526104</v>
+      </c>
+      <c r="E40">
+        <v>14.295632913051501</v>
+      </c>
+      <c r="F40">
+        <v>14.1</v>
+      </c>
+      <c r="G40">
+        <v>4.36444393742938</v>
+      </c>
+      <c r="H40" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>59</v>
+      </c>
+      <c r="B41">
+        <v>15.193930115608</v>
+      </c>
+      <c r="C41">
+        <v>15.2</v>
+      </c>
+      <c r="D41">
+        <v>4.0991775771240002</v>
+      </c>
+      <c r="E41">
+        <v>16.330161561057501</v>
+      </c>
+      <c r="F41">
+        <v>16.2</v>
+      </c>
+      <c r="G41">
+        <v>4.1802344760786196</v>
+      </c>
+      <c r="H41" s="14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified regression tree models in data 2016
</commit_message>
<xml_diff>
--- a/output/resultsummary.xlsx
+++ b/output/resultsummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yzz3363/Documents/Rstudio/UBRR/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D96E52-4478-7C43-A150-B18126EE0BED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F03EC5-5938-214A-87C1-89720031EA4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{A4114632-EF87-9B4A-9301-938BFB9B362C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{A4114632-EF87-9B4A-9301-938BFB9B362C}"/>
   </bookViews>
   <sheets>
     <sheet name="2014" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="61">
   <si>
     <t>Urban</t>
   </si>
@@ -283,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -299,6 +299,8 @@
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB45659A-0F08-1C42-BDBF-A87EBD364EFE}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="106" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -1706,7 +1708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDB2D81-59B2-0D49-B33A-5E9C030744C6}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="142" workbookViewId="0">
+    <sheetView zoomScale="83" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -2545,10 +2547,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E07747-FDDA-4847-BAEB-2E4FAA0F34D2}">
-  <dimension ref="A2:A40"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A40"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2556,180 +2558,725 @@
     <col min="1" max="1" width="45.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>83</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="D2">
+        <v>140</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>400</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D3">
+        <v>2111</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>747</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D4">
+        <v>4126</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>4234</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.1E-2</v>
+      </c>
+      <c r="D5">
+        <v>4007</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <v>6830</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D6">
+        <v>4578</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>3384</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="D7">
+        <v>2016</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>122882</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="D8">
+        <v>22858</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.57399999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>138560</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>39836</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="B14">
+        <v>134622</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="D14">
+        <v>38928</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.97699999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15">
+        <v>131411</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="D15">
+        <v>35264</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.88500000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="14">
+        <v>125808</v>
+      </c>
+      <c r="C16" s="16">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="D16">
+        <v>33599</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.84299999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>122697</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="D17" s="8">
+        <v>28969</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0.72699999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B18">
+        <v>131984</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="D18" s="14">
+        <v>38361</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0.96299999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="14">
+        <v>3.2737545696000301</v>
+      </c>
+      <c r="C21" s="14">
+        <v>3.5</v>
+      </c>
+      <c r="D21" s="14">
+        <v>0.92519788898423905</v>
+      </c>
+      <c r="E21" s="14">
+        <v>3.23298527752871</v>
+      </c>
+      <c r="F21" s="14">
+        <v>3</v>
+      </c>
+      <c r="G21" s="14">
+        <v>0.85710011432004696</v>
+      </c>
+      <c r="H21" s="12">
+        <v>3.2541972231620603E-20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B22" s="8">
+        <v>91.6068362079819</v>
+      </c>
+      <c r="C22" s="8">
+        <v>94.5</v>
+      </c>
+      <c r="D22" s="8">
+        <v>9.0468804975097701</v>
+      </c>
+      <c r="E22" s="5">
+        <v>93.135625957539901</v>
+      </c>
+      <c r="F22" s="5">
+        <v>95.2</v>
+      </c>
+      <c r="G22" s="5">
+        <v>6.9489779771586502</v>
+      </c>
+      <c r="H22" s="12">
+        <v>1.8343283028903E-84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B23" s="14">
+        <v>95.610264563609704</v>
+      </c>
+      <c r="C23" s="14">
+        <v>98.4</v>
+      </c>
+      <c r="D23" s="14">
+        <v>8.5972774107461802</v>
+      </c>
+      <c r="E23" s="14">
+        <v>95.543441949616593</v>
+      </c>
+      <c r="F23" s="14">
+        <v>98.3</v>
+      </c>
+      <c r="G23" s="14">
+        <v>7.8500807390706004</v>
+      </c>
+      <c r="H23" s="12">
+        <v>2.3642007249685102E-15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B24" s="15">
+        <v>99.127516363401398</v>
+      </c>
+      <c r="C24" s="15">
+        <v>100</v>
+      </c>
+      <c r="D24" s="15">
+        <v>2.9467684787866499</v>
+      </c>
+      <c r="E24" s="15">
+        <v>99.250459095045102</v>
+      </c>
+      <c r="F24" s="15">
+        <v>100</v>
+      </c>
+      <c r="G24" s="15">
+        <v>2.85301043743535</v>
+      </c>
+      <c r="H24" s="13">
+        <v>0.22715474904372299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B25" s="8">
+        <v>96.382472471029203</v>
+      </c>
+      <c r="C25" s="8">
+        <v>99.1</v>
+      </c>
+      <c r="D25" s="8">
+        <v>9.0277581088831695</v>
+      </c>
+      <c r="E25" s="5">
+        <v>97.427860955248406</v>
+      </c>
+      <c r="F25" s="5">
+        <v>99.2</v>
+      </c>
+      <c r="G25" s="5">
+        <v>6.0492998199408099</v>
+      </c>
+      <c r="H25" s="12">
+        <v>6.95244220159194E-9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B26" s="14">
+        <v>69.327898696699094</v>
+      </c>
+      <c r="C26" s="14">
+        <v>74.7</v>
+      </c>
+      <c r="D26" s="14">
+        <v>21.2743722958128</v>
+      </c>
+      <c r="E26" s="14">
+        <v>72.843367890165297</v>
+      </c>
+      <c r="F26" s="14">
+        <v>75</v>
+      </c>
+      <c r="G26" s="14">
+        <v>14.2246999034379</v>
+      </c>
+      <c r="H26" s="12">
+        <v>7.3082788337868905E-19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B27" s="14">
+        <v>71.171411001889993</v>
+      </c>
+      <c r="C27" s="14">
+        <v>78.7</v>
+      </c>
+      <c r="D27" s="14">
+        <v>24.060951461446201</v>
+      </c>
+      <c r="E27" s="14">
+        <v>78.617102737096204</v>
+      </c>
+      <c r="F27" s="14">
+        <v>82.2</v>
+      </c>
+      <c r="G27" s="14">
+        <v>15.587584375677199</v>
+      </c>
+      <c r="H27" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B28" s="8">
+        <v>96.277454009846906</v>
+      </c>
+      <c r="C28" s="8">
+        <v>98.8</v>
+      </c>
+      <c r="D28" s="8">
+        <v>7.7409667481147304</v>
+      </c>
+      <c r="E28" s="14">
+        <v>96.017297622630196</v>
+      </c>
+      <c r="F28" s="14">
+        <v>98.5</v>
+      </c>
+      <c r="G28" s="14">
+        <v>7.3390648164698602</v>
+      </c>
+      <c r="H28" s="12">
+        <v>1.52425495601471E-55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B29" s="14">
+        <v>76.607781132000298</v>
+      </c>
+      <c r="C29" s="14">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="D29" s="14">
+        <v>17.334041420254799</v>
+      </c>
+      <c r="E29" s="14">
+        <v>77.388780330369997</v>
+      </c>
+      <c r="F29" s="14">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="G29" s="14">
+        <v>15.274128963630901</v>
+      </c>
+      <c r="H29" s="14">
+        <v>4.5085951612506602E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="B30" s="14">
+        <v>74.543542177806998</v>
+      </c>
+      <c r="C30" s="14">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D30" s="14">
+        <v>19.383760504136099</v>
+      </c>
+      <c r="E30" s="14">
+        <v>76.262326574172903</v>
+      </c>
+      <c r="F30" s="14">
+        <v>75.2</v>
+      </c>
+      <c r="G30" s="14">
+        <v>16.913723142874499</v>
+      </c>
+      <c r="H30" s="12">
+        <v>1.63851417754219E-23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B31" s="13">
+        <v>79.0263579799214</v>
+      </c>
+      <c r="C31" s="13">
+        <v>80.2</v>
+      </c>
+      <c r="D31" s="13">
+        <v>17.924847056398601</v>
+      </c>
+      <c r="E31" s="13">
+        <v>79.749146185537697</v>
+      </c>
+      <c r="F31" s="13">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="G31" s="13">
+        <v>15.610603611001499</v>
+      </c>
+      <c r="H31" s="13">
+        <v>3.8901155284036003E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B32" s="14">
+        <v>70.814630533114695</v>
+      </c>
+      <c r="C32" s="14">
+        <v>72.2</v>
+      </c>
+      <c r="D32" s="14">
+        <v>17.895268936644602</v>
+      </c>
+      <c r="E32" s="14">
+        <v>68.266121950510296</v>
+      </c>
+      <c r="F32" s="14">
+        <v>68.8</v>
+      </c>
+      <c r="G32" s="14">
+        <v>14.692079707323</v>
+      </c>
+      <c r="H32" s="12">
+        <v>1.16600699572607E-237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="B33" s="13">
+        <v>66.197692176306902</v>
+      </c>
+      <c r="C33" s="13">
+        <v>69.3</v>
+      </c>
+      <c r="D33" s="13">
+        <v>19.153630049053199</v>
+      </c>
+      <c r="E33" s="13">
+        <v>66.819908683921895</v>
+      </c>
+      <c r="F33" s="13">
+        <v>68.8</v>
+      </c>
+      <c r="G33" s="13">
+        <v>15.8202528894442</v>
+      </c>
+      <c r="H33" s="13">
+        <v>1.50357609764527E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B34" s="14">
+        <v>80.084340682370694</v>
+      </c>
+      <c r="C34" s="14">
+        <v>85.5</v>
+      </c>
+      <c r="D34" s="14">
+        <v>17.040683385713098</v>
+      </c>
+      <c r="E34" s="14">
+        <v>81.931078678629007</v>
+      </c>
+      <c r="F34" s="14">
+        <v>87.3</v>
+      </c>
+      <c r="G34" s="14">
+        <v>15.1502359352681</v>
+      </c>
+      <c r="H34" s="12">
+        <v>3.9113939311179499E-28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B35" s="14">
+        <v>57.205597526088901</v>
+      </c>
+      <c r="C35" s="14">
+        <v>58.3</v>
+      </c>
+      <c r="D35" s="14">
+        <v>16.732696648741499</v>
+      </c>
+      <c r="E35" s="14">
+        <v>58.154274055627198</v>
+      </c>
+      <c r="F35" s="14">
+        <v>58.5</v>
+      </c>
+      <c r="G35" s="14">
+        <v>13.8536730252605</v>
+      </c>
+      <c r="H35" s="12">
+        <v>3.1061247513897799E-9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B36" s="14">
+        <v>15.2430413428268</v>
+      </c>
+      <c r="C36" s="14">
+        <v>15.3</v>
+      </c>
+      <c r="D36" s="14">
+        <v>4.0957201019779204</v>
+      </c>
+      <c r="E36" s="14">
+        <v>16.329583668124901</v>
+      </c>
+      <c r="F36" s="14">
+        <v>16.2</v>
+      </c>
+      <c r="G36" s="14">
+        <v>4.1539593495062102</v>
+      </c>
+      <c r="H36" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
         <v>59</v>
       </c>
+      <c r="B37" s="14">
+        <v>11.9162227501104</v>
+      </c>
+      <c r="C37" s="14">
+        <v>11.8</v>
+      </c>
+      <c r="D37" s="14">
+        <v>4.1174353071794796</v>
+      </c>
+      <c r="E37" s="14">
+        <v>14.352468474898901</v>
+      </c>
+      <c r="F37" s="14">
+        <v>14.2</v>
+      </c>
+      <c r="G37" s="14">
+        <v>4.3391086088634498</v>
+      </c>
+      <c r="H37" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="10"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>